<commit_message>
Made some minor fixes to raw data files.
</commit_message>
<xml_diff>
--- a/data/IDsheet.xlsx
+++ b/data/IDsheet.xlsx
@@ -17,9 +17,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="12">
-  <si>
-    <t>ID</t>
-  </si>
   <si>
     <t>Cond</t>
   </si>
@@ -52,6 +49,9 @@
   </si>
   <si>
     <t>A</t>
+  </si>
+  <si>
+    <t>Subject</t>
   </si>
 </sst>
 </file>
@@ -385,27 +385,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -413,10 +413,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -424,10 +424,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -435,13 +435,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -449,13 +449,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -463,10 +463,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -474,13 +474,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -488,10 +488,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -499,10 +499,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -510,10 +510,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -521,13 +521,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -535,10 +535,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -546,10 +546,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -557,10 +557,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -568,13 +568,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -582,10 +582,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -593,10 +593,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -604,13 +604,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -618,10 +618,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -629,10 +629,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -640,10 +640,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -651,10 +651,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -662,10 +662,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -673,13 +673,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -687,10 +687,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -698,10 +698,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -709,13 +709,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -723,10 +723,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -734,13 +734,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -748,10 +748,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -759,10 +759,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -770,10 +770,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -781,10 +781,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -792,13 +792,13 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -806,10 +806,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -817,10 +817,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -828,10 +828,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C37" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -839,10 +839,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -850,10 +850,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -861,10 +861,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -872,10 +872,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C41" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -883,10 +883,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -894,10 +894,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C43" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -905,10 +905,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -916,10 +916,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -927,10 +927,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -938,10 +938,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C47" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -949,10 +949,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C48" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -960,10 +960,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C49" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -971,10 +971,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C50" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -982,10 +982,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C51" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -993,10 +993,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C52" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1004,10 +1004,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C53" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1015,10 +1015,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C54" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1026,13 +1026,13 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C55" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D55" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1040,13 +1040,13 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C56" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D56" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1054,13 +1054,13 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C57" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D57" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -1068,13 +1068,13 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C58" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D58" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -1082,13 +1082,13 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C59" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D59" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -1096,13 +1096,13 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C60" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D60" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -1110,13 +1110,13 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C61" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D61" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -1124,13 +1124,13 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C62" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D62" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -1138,13 +1138,13 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C63" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D63" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -1152,16 +1152,16 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C64" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D64" t="s">
+        <v>9</v>
+      </c>
+      <c r="E64" t="s">
         <v>10</v>
-      </c>
-      <c r="E64" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -1169,13 +1169,13 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C65" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D65" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -1183,16 +1183,16 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C66" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D66" t="s">
+        <v>9</v>
+      </c>
+      <c r="E66" t="s">
         <v>10</v>
-      </c>
-      <c r="E66" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>